<commit_message>
Align with tables in Supplementary Material
</commit_message>
<xml_diff>
--- a/data-sources/CMIP5_simulations_ATLAS.xlsx
+++ b/data-sources/CMIP5_simulations_ATLAS.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gutierjm/Desktop/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gutierjm/_IPCC-AR6/FGD/_InteractiveAtlas/_simulations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F050C6C7-D479-8948-824A-1B383F9545F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18C42B6-D0EF-4344-BBC2-5AA04283CB83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9440" yWindow="460" windowWidth="22260" windowHeight="20120" xr2:uid="{8437F848-4E77-4E44-A82D-3C2AC1293F55}"/>
+    <workbookView xWindow="5680" yWindow="1280" windowWidth="25860" windowHeight="17120" xr2:uid="{8437F848-4E77-4E44-A82D-3C2AC1293F55}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="71">
   <si>
     <t>RCP2.6</t>
   </si>
@@ -61,27 +61,6 @@
         <rFont val="Calibri (Cuerpo)"/>
       </rPr>
       <t>P T X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>P X</t>
     </r>
     <r>
       <rPr>
@@ -279,12 +258,111 @@
   <si>
     <t xml:space="preserve">Fixed fields - E: elevation (orog), L: land/sea mask (ssftlf) in the historical scenario </t>
   </si>
+  <si>
+    <t>Discarded (no temperature in projections)</t>
+  </si>
+  <si>
+    <t>No pre-Industrial data (no global warming levles)</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
+    <t>https://pcmdi.llnl.gov/mips/cmip5/availability.html</t>
+  </si>
+  <si>
+    <t>CCCma</t>
+  </si>
+  <si>
+    <t>CMCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CNRM-CERFACS</t>
+  </si>
+  <si>
+    <t>CSIRO-BOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CSIRO-QCCCE</t>
+  </si>
+  <si>
+    <t>IPSL</t>
+  </si>
+  <si>
+    <t>INM</t>
+  </si>
+  <si>
+    <t>MIROC</t>
+  </si>
+  <si>
+    <t>MOHC </t>
+  </si>
+  <si>
+    <t>MPI-M</t>
+  </si>
+  <si>
+    <t>MRI</t>
+  </si>
+  <si>
+    <t>NOAA GFDL</t>
+  </si>
+  <si>
+    <t>LASG-CESS</t>
+  </si>
+  <si>
+    <t>NCAR</t>
+  </si>
+  <si>
+    <t>NSF-DOE-NCAR</t>
+  </si>
+  <si>
+    <t>GCESS</t>
+  </si>
+  <si>
+    <t>NCC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>P T X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>P X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -313,6 +391,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -337,10 +450,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -367,8 +481,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -681,14 +807,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8382EADB-5382-9C44-BAB4-9F72AA75DD74}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
@@ -699,10 +827,10 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1">
       <c r="A1" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -723,21 +851,24 @@
         <v>2</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>6</v>
@@ -749,18 +880,22 @@
         <v>6</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>6</v>
@@ -772,18 +907,22 @@
         <v>6</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>6</v>
@@ -798,18 +937,22 @@
         <v>6</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>6</v>
@@ -823,16 +966,20 @@
       <c r="H5" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>6</v>
@@ -847,18 +994,24 @@
         <v>6</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>6</v>
@@ -873,18 +1026,22 @@
         <v>6</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>6</v>
@@ -899,18 +1056,22 @@
         <v>6</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>6</v>
@@ -922,18 +1083,22 @@
         <v>6</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>6</v>
@@ -945,18 +1110,22 @@
         <v>6</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>6</v>
@@ -968,18 +1137,22 @@
         <v>6</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>6</v>
@@ -994,18 +1167,22 @@
         <v>6</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>6</v>
@@ -1020,67 +1197,78 @@
         <v>6</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
         <v>25</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" s="14" customFormat="1">
+      <c r="B15" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>46</v>
+      <c r="D15" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>6</v>
@@ -1092,18 +1280,22 @@
         <v>6</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>6</v>
@@ -1118,18 +1310,22 @@
         <v>6</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>6</v>
@@ -1144,18 +1340,22 @@
         <v>6</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>6</v>
@@ -1167,18 +1367,22 @@
         <v>6</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>6</v>
@@ -1193,18 +1397,22 @@
         <v>6</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>6</v>
@@ -1216,21 +1424,24 @@
         <v>6</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" t="s">
-        <v>9</v>
+        <v>45</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>6</v>
@@ -1245,18 +1456,22 @@
         <v>6</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>6</v>
@@ -1271,18 +1486,22 @@
         <v>6</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>6</v>
@@ -1294,18 +1513,22 @@
         <v>6</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>6</v>
@@ -1320,18 +1543,22 @@
         <v>6</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>6</v>
@@ -1346,18 +1573,22 @@
         <v>6</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>6</v>
@@ -1372,18 +1603,22 @@
         <v>6</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>6</v>
@@ -1398,18 +1633,22 @@
         <v>6</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J28" s="10"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>6</v>
@@ -1424,18 +1663,22 @@
         <v>6</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J29" s="10"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>6</v>
@@ -1450,18 +1693,22 @@
         <v>6</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J30" s="10"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>6</v>
@@ -1476,24 +1723,25 @@
         <v>6</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J31" s="10"/>
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="4"/>
       <c r="I33" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="2:9">
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -1501,7 +1749,15 @@
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
     </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B36" r:id="rId1" xr:uid="{80916A6F-30C5-4249-8673-F4E0C08F1565}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>